<commit_message>
edit optimisation files for shap and rf selected features. added Clinical A and C optimization for top features
</commit_message>
<xml_diff>
--- a/Optimisation data/combined/Biomarkers + Clinical A/top/RF_feature_importance/LogisticRegression_optimisation.xlsx
+++ b/Optimisation data/combined/Biomarkers + Clinical A/top/RF_feature_importance/LogisticRegression_optimisation.xlsx
@@ -157,7 +157,7 @@
     <t>{'C': 1.0, 'class_weight': None, 'dual': False, 'fit_intercept': False, 'max_iter': 10000, 'multi_class': 'auto', 'penalty': 'none', 'random_state': 10, 'tol': 0.0001, 'verbose': 0, 'warm_start': True}</t>
   </si>
   <si>
-    <t>[0.66507177 0.52631579 0.59808612 0.83732057 0.555     ]</t>
+    <t>[0.66985646 0.64114833 0.54066986 0.60287081 0.67      ]</t>
   </si>
 </sst>
 </file>
@@ -609,16 +609,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.009986114501953126</v>
+        <v>0.004255390167236328</v>
       </c>
       <c r="C2">
-        <v>0.006386433652011925</v>
+        <v>0.002134899894764335</v>
       </c>
       <c r="D2">
-        <v>0.003919219970703125</v>
+        <v>0.001120805740356445</v>
       </c>
       <c r="E2">
-        <v>0.002337721674697482</v>
+        <v>0.0002697294199972461</v>
       </c>
       <c r="F2">
         <v>0.001</v>
@@ -657,37 +657,37 @@
         <v>31</v>
       </c>
       <c r="R2">
-        <v>0.4137931034482759</v>
+        <v>0.7</v>
       </c>
       <c r="S2">
-        <v>0.5</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="T2">
-        <v>0.5333333333333333</v>
+        <v>0.5405405405405405</v>
       </c>
       <c r="U2">
-        <v>0.4285714285714285</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="V2">
-        <v>0.631578947368421</v>
+        <v>0.6666666666666665</v>
       </c>
       <c r="W2">
-        <v>0.5014553625442917</v>
+        <v>0.6647747747747748</v>
       </c>
       <c r="X2">
-        <v>0.0786730067182161</v>
+        <v>0.06920326433411365</v>
       </c>
       <c r="Y2">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="Z2" t="s">
         <v>47</v>
       </c>
       <c r="AA2">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB2">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -695,16 +695,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.009130096435546875</v>
+        <v>0.003809595108032227</v>
       </c>
       <c r="C3">
-        <v>0.002961322544930611</v>
+        <v>0.001804851336569589</v>
       </c>
       <c r="D3">
-        <v>0.002693462371826172</v>
+        <v>0.0009220600128173828</v>
       </c>
       <c r="E3">
-        <v>0.002703472351645345</v>
+        <v>0.0001166264733287864</v>
       </c>
       <c r="F3">
         <v>0.001</v>
@@ -743,37 +743,37 @@
         <v>32</v>
       </c>
       <c r="R3">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="S3">
-        <v>0.6285714285714286</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T3">
-        <v>0.6060606060606061</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="U3">
-        <v>0.6206896551724138</v>
+        <v>0.5161290322580646</v>
       </c>
       <c r="V3">
-        <v>0.6666666666666667</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="W3">
-        <v>0.6301119570085086</v>
+        <v>0.5818708353133599</v>
       </c>
       <c r="X3">
-        <v>0.02004116018713882</v>
+        <v>0.08078338181691065</v>
       </c>
       <c r="Y3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z3" t="s">
         <v>47</v>
       </c>
       <c r="AA3">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB3">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -781,16 +781,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.004013347625732422</v>
+        <v>0.001779794692993164</v>
       </c>
       <c r="C4">
-        <v>0.00143142618816301</v>
+        <v>0.001009151129071246</v>
       </c>
       <c r="D4">
-        <v>0.003042745590209961</v>
+        <v>0.0008942127227783203</v>
       </c>
       <c r="E4">
-        <v>0.002158519096964711</v>
+        <v>0.0004473625533180876</v>
       </c>
       <c r="F4">
         <v>0.001</v>
@@ -826,37 +826,37 @@
         <v>33</v>
       </c>
       <c r="R4">
-        <v>0.6666666666666667</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="S4">
-        <v>0.6666666666666667</v>
+        <v>0.7804878048780488</v>
       </c>
       <c r="T4">
-        <v>0.5945945945945946</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="U4">
-        <v>0.6829268292682926</v>
+        <v>0.7027027027027027</v>
       </c>
       <c r="V4">
-        <v>0.6</v>
+        <v>0.7692307692307692</v>
       </c>
       <c r="W4">
-        <v>0.6421709514392442</v>
+        <v>0.7291809972169407</v>
       </c>
       <c r="X4">
-        <v>0.03715648148714518</v>
+        <v>0.05573953308217269</v>
       </c>
       <c r="Y4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="s">
         <v>47</v>
       </c>
       <c r="AA4">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB4">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -864,16 +864,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.003403282165527344</v>
+        <v>0.00194544792175293</v>
       </c>
       <c r="C5">
-        <v>0.001959471678433925</v>
+        <v>0.0005363525825055996</v>
       </c>
       <c r="D5">
-        <v>0.0009590625762939453</v>
+        <v>0.001091480255126953</v>
       </c>
       <c r="E5">
-        <v>0.0003090678665595652</v>
+        <v>0.0007875697058363001</v>
       </c>
       <c r="F5">
         <v>0.001</v>
@@ -909,37 +909,37 @@
         <v>34</v>
       </c>
       <c r="R5">
-        <v>0.7027027027027027</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="S5">
-        <v>0.6486486486486486</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="T5">
-        <v>0.6666666666666667</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="U5">
-        <v>0.7096774193548387</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="V5">
-        <v>0.7</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="W5">
-        <v>0.6855390874745714</v>
+        <v>0.6583072753804462</v>
       </c>
       <c r="X5">
-        <v>0.02367884916396554</v>
+        <v>0.06624626274899952</v>
       </c>
       <c r="Y5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Z5" t="s">
         <v>47</v>
       </c>
       <c r="AA5">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB5">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -947,16 +947,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.004490852355957031</v>
+        <v>0.002114534378051758</v>
       </c>
       <c r="C6">
-        <v>0.001784403885601361</v>
+        <v>0.001056559135856211</v>
       </c>
       <c r="D6">
-        <v>0.001984882354736328</v>
+        <v>0.0008840560913085938</v>
       </c>
       <c r="E6">
-        <v>0.0006105738734154246</v>
+        <v>0.0003701165360454291</v>
       </c>
       <c r="F6">
         <v>0.01</v>
@@ -995,37 +995,37 @@
         <v>35</v>
       </c>
       <c r="R6">
-        <v>0.5882352941176471</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="S6">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="T6">
-        <v>0.6</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="U6">
-        <v>0.4615384615384616</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="V6">
-        <v>0.631578947368421</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="W6">
-        <v>0.5819848263191917</v>
+        <v>0.6829381145170619</v>
       </c>
       <c r="X6">
-        <v>0.06245130898771563</v>
+        <v>0.03197673360754662</v>
       </c>
       <c r="Y6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="Z6" t="s">
         <v>47</v>
       </c>
       <c r="AA6">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB6">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -1033,16 +1033,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.003664398193359375</v>
+        <v>0.00311436653137207</v>
       </c>
       <c r="C7">
-        <v>0.001064374160185618</v>
+        <v>0.001747063969683034</v>
       </c>
       <c r="D7">
-        <v>0.001093626022338867</v>
+        <v>0.0007877349853515625</v>
       </c>
       <c r="E7">
-        <v>0.0002398190849297886</v>
+        <v>0.0001448485779627544</v>
       </c>
       <c r="F7">
         <v>0.01</v>
@@ -1081,37 +1081,37 @@
         <v>36</v>
       </c>
       <c r="R7">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="S7">
-        <v>0.6285714285714286</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T7">
-        <v>0.6060606060606061</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="U7">
-        <v>0.6206896551724138</v>
+        <v>0.5161290322580646</v>
       </c>
       <c r="V7">
-        <v>0.6666666666666667</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="W7">
-        <v>0.6301119570085086</v>
+        <v>0.5818708353133599</v>
       </c>
       <c r="X7">
-        <v>0.02004116018713882</v>
+        <v>0.08078338181691065</v>
       </c>
       <c r="Y7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z7" t="s">
         <v>47</v>
       </c>
       <c r="AA7">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB7">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -1119,16 +1119,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.002155017852783203</v>
+        <v>0.00181884765625</v>
       </c>
       <c r="C8">
-        <v>0.0004005883793115504</v>
+        <v>0.0008195693556861795</v>
       </c>
       <c r="D8">
-        <v>0.000939035415649414</v>
+        <v>0.0007009506225585938</v>
       </c>
       <c r="E8">
-        <v>0.0001788245897297263</v>
+        <v>7.711593565371269E-05</v>
       </c>
       <c r="F8">
         <v>0.01</v>
@@ -1164,37 +1164,37 @@
         <v>37</v>
       </c>
       <c r="R8">
-        <v>0.6857142857142857</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="S8">
-        <v>0.6842105263157895</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="T8">
-        <v>0.631578947368421</v>
+        <v>0.6500000000000001</v>
       </c>
       <c r="U8">
-        <v>0.6666666666666667</v>
+        <v>0.7027027027027027</v>
       </c>
       <c r="V8">
-        <v>0.6153846153846154</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="W8">
-        <v>0.6567110082899558</v>
+        <v>0.7093683793683795</v>
       </c>
       <c r="X8">
-        <v>0.02841133563720606</v>
+        <v>0.03585222335390306</v>
       </c>
       <c r="Y8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Z8" t="s">
         <v>47</v>
       </c>
       <c r="AA8">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB8">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -1202,16 +1202,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.005538225173950195</v>
+        <v>0.001537609100341797</v>
       </c>
       <c r="C9">
-        <v>0.00225293593114248</v>
+        <v>0.0001937005859222918</v>
       </c>
       <c r="D9">
-        <v>0.002800559997558594</v>
+        <v>0.0006522655487060547</v>
       </c>
       <c r="E9">
-        <v>0.0008194961828547688</v>
+        <v>3.259013666245423E-05</v>
       </c>
       <c r="F9">
         <v>0.01</v>
@@ -1247,37 +1247,37 @@
         <v>38</v>
       </c>
       <c r="R9">
-        <v>0.7027027027027027</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="S9">
-        <v>0.6486486486486486</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="T9">
-        <v>0.6666666666666667</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="U9">
-        <v>0.7096774193548387</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="V9">
-        <v>0.7</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="W9">
-        <v>0.6855390874745714</v>
+        <v>0.6583072753804462</v>
       </c>
       <c r="X9">
-        <v>0.02367884916396554</v>
+        <v>0.06624626274899952</v>
       </c>
       <c r="Y9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Z9" t="s">
         <v>47</v>
       </c>
       <c r="AA9">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB9">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -1285,16 +1285,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.01060762405395508</v>
+        <v>0.001807165145874023</v>
       </c>
       <c r="C10">
-        <v>0.003744457578592539</v>
+        <v>0.0001513579388838597</v>
       </c>
       <c r="D10">
-        <v>0.005328798294067382</v>
+        <v>0.0007008075714111328</v>
       </c>
       <c r="E10">
-        <v>0.003972385109299549</v>
+        <v>4.664057321818651E-05</v>
       </c>
       <c r="F10">
         <v>0.1</v>
@@ -1333,37 +1333,37 @@
         <v>39</v>
       </c>
       <c r="R10">
-        <v>0.6285714285714286</v>
+        <v>0.7567567567567567</v>
       </c>
       <c r="S10">
-        <v>0.6470588235294117</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T10">
-        <v>0.625</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="U10">
-        <v>0.6206896551724138</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="V10">
-        <v>0.631578947368421</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="W10">
-        <v>0.6305797709283351</v>
+        <v>0.607764427051354</v>
       </c>
       <c r="X10">
-        <v>0.00900598912378016</v>
+        <v>0.08362456130537084</v>
       </c>
       <c r="Y10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Z10" t="s">
         <v>47</v>
       </c>
       <c r="AA10">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB10">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -1371,16 +1371,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.01032400131225586</v>
+        <v>0.001755952835083008</v>
       </c>
       <c r="C11">
-        <v>0.004752748805612586</v>
+        <v>0.0002532565599078225</v>
       </c>
       <c r="D11">
-        <v>0.004078388214111328</v>
+        <v>0.000637674331665039</v>
       </c>
       <c r="E11">
-        <v>0.003543352811159192</v>
+        <v>2.436381249994812E-05</v>
       </c>
       <c r="F11">
         <v>0.1</v>
@@ -1419,37 +1419,37 @@
         <v>40</v>
       </c>
       <c r="R11">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="S11">
-        <v>0.6285714285714286</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T11">
-        <v>0.6060606060606061</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="U11">
-        <v>0.6206896551724138</v>
+        <v>0.5161290322580646</v>
       </c>
       <c r="V11">
-        <v>0.6666666666666667</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="W11">
-        <v>0.6301119570085086</v>
+        <v>0.5818708353133599</v>
       </c>
       <c r="X11">
-        <v>0.02004116018713882</v>
+        <v>0.08078338181691065</v>
       </c>
       <c r="Y11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z11" t="s">
         <v>47</v>
       </c>
       <c r="AA11">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB11">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -1457,16 +1457,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.005327463150024414</v>
+        <v>0.001327180862426758</v>
       </c>
       <c r="C12">
-        <v>0.002587708723400833</v>
+        <v>0.0001795394547505557</v>
       </c>
       <c r="D12">
-        <v>0.001940679550170898</v>
+        <v>0.0006309032440185546</v>
       </c>
       <c r="E12">
-        <v>0.0009524281036413114</v>
+        <v>3.041548340657028E-05</v>
       </c>
       <c r="F12">
         <v>0.1</v>
@@ -1502,37 +1502,37 @@
         <v>41</v>
       </c>
       <c r="R12">
-        <v>0.7027027027027027</v>
+        <v>0.7804878048780488</v>
       </c>
       <c r="S12">
-        <v>0.6486486486486486</v>
+        <v>0.7</v>
       </c>
       <c r="T12">
-        <v>0.6842105263157895</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="U12">
-        <v>0.7499999999999999</v>
+        <v>0.742857142857143</v>
       </c>
       <c r="V12">
-        <v>0.6829268292682926</v>
+        <v>0.7</v>
       </c>
       <c r="W12">
-        <v>0.6936977413870867</v>
+        <v>0.7004584632312488</v>
       </c>
       <c r="X12">
-        <v>0.03312544100067901</v>
+        <v>0.06777567424597226</v>
       </c>
       <c r="Y12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z12" t="s">
         <v>47</v>
       </c>
       <c r="AA12">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB12">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -1540,16 +1540,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.00400700569152832</v>
+        <v>0.001394176483154297</v>
       </c>
       <c r="C13">
-        <v>0.00129919147505421</v>
+        <v>0.0001151481866534802</v>
       </c>
       <c r="D13">
-        <v>0.002137374877929687</v>
+        <v>0.0006142616271972656</v>
       </c>
       <c r="E13">
-        <v>0.001250375834603681</v>
+        <v>1.116919158975634E-05</v>
       </c>
       <c r="F13">
         <v>0.1</v>
@@ -1585,37 +1585,37 @@
         <v>42</v>
       </c>
       <c r="R13">
-        <v>0.7027027027027027</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="S13">
-        <v>0.6486486486486486</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="T13">
-        <v>0.6666666666666667</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="U13">
-        <v>0.7096774193548387</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="V13">
-        <v>0.7</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="W13">
-        <v>0.6855390874745714</v>
+        <v>0.6583072753804462</v>
       </c>
       <c r="X13">
-        <v>0.02367884916396554</v>
+        <v>0.06624626274899952</v>
       </c>
       <c r="Y13">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Z13" t="s">
         <v>47</v>
       </c>
       <c r="AA13">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB13">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="14" spans="1:28">
@@ -1623,16 +1623,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.003086471557617188</v>
+        <v>0.002327537536621094</v>
       </c>
       <c r="C14">
-        <v>0.0007670003225369225</v>
+        <v>0.001164663583200146</v>
       </c>
       <c r="D14">
-        <v>0.002457380294799805</v>
+        <v>0.0009757041931152344</v>
       </c>
       <c r="E14">
-        <v>0.001442307521994305</v>
+        <v>0.0007048918993664734</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1671,37 +1671,37 @@
         <v>43</v>
       </c>
       <c r="R14">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="S14">
-        <v>0.6285714285714286</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T14">
-        <v>0.6060606060606061</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="U14">
-        <v>0.6206896551724138</v>
+        <v>0.5161290322580646</v>
       </c>
       <c r="V14">
-        <v>0.631578947368421</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="W14">
-        <v>0.6230944131488595</v>
+        <v>0.5818708353133599</v>
       </c>
       <c r="X14">
-        <v>0.009251120598566864</v>
+        <v>0.08078338181691065</v>
       </c>
       <c r="Y14">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Z14" t="s">
         <v>47</v>
       </c>
       <c r="AA14">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB14">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="15" spans="1:28">
@@ -1709,16 +1709,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.006169414520263672</v>
+        <v>0.002364253997802734</v>
       </c>
       <c r="C15">
-        <v>0.002049528583368748</v>
+        <v>0.001008450657391694</v>
       </c>
       <c r="D15">
-        <v>0.006886863708496093</v>
+        <v>0.0006611347198486328</v>
       </c>
       <c r="E15">
-        <v>0.002793934384999051</v>
+        <v>8.830568433664599E-05</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1757,37 +1757,37 @@
         <v>44</v>
       </c>
       <c r="R15">
-        <v>0.6285714285714286</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="S15">
-        <v>0.6285714285714286</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="T15">
-        <v>0.6060606060606061</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="U15">
-        <v>0.6206896551724138</v>
+        <v>0.5161290322580646</v>
       </c>
       <c r="V15">
-        <v>0.6666666666666667</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="W15">
-        <v>0.6301119570085086</v>
+        <v>0.5818708353133599</v>
       </c>
       <c r="X15">
-        <v>0.02004116018713882</v>
+        <v>0.08078338181691065</v>
       </c>
       <c r="Y15">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z15" t="s">
         <v>47</v>
       </c>
       <c r="AA15">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB15">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -1795,16 +1795,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.006197690963745117</v>
+        <v>0.001373100280761719</v>
       </c>
       <c r="C16">
-        <v>0.00288585141154333</v>
+        <v>0.0001090106895864201</v>
       </c>
       <c r="D16">
-        <v>0.002931404113769531</v>
+        <v>0.0006118297576904296</v>
       </c>
       <c r="E16">
-        <v>0.001144534674359913</v>
+        <v>1.415523852669371E-05</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1840,37 +1840,37 @@
         <v>45</v>
       </c>
       <c r="R16">
-        <v>0.7027027027027027</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="S16">
-        <v>0.6486486486486486</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="T16">
-        <v>0.6666666666666667</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="U16">
-        <v>0.7096774193548387</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="V16">
-        <v>0.7</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="W16">
-        <v>0.6855390874745714</v>
+        <v>0.6652046783625731</v>
       </c>
       <c r="X16">
-        <v>0.02367884916396554</v>
+        <v>0.06869789546474113</v>
       </c>
       <c r="Y16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z16" t="s">
         <v>47</v>
       </c>
       <c r="AA16">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB16">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -1878,16 +1878,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.003284692764282227</v>
+        <v>0.001378250122070313</v>
       </c>
       <c r="C17">
-        <v>0.001800181056385022</v>
+        <v>0.0001031700196930825</v>
       </c>
       <c r="D17">
-        <v>0.001909732818603516</v>
+        <v>0.0006153583526611328</v>
       </c>
       <c r="E17">
-        <v>0.001076119407087371</v>
+        <v>1.802734573671376E-05</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1923,37 +1923,37 @@
         <v>46</v>
       </c>
       <c r="R17">
-        <v>0.7027027027027027</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="S17">
-        <v>0.6486486486486486</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="T17">
-        <v>0.6666666666666667</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="U17">
-        <v>0.7096774193548387</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="V17">
-        <v>0.7</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="W17">
-        <v>0.6855390874745714</v>
+        <v>0.6583072753804462</v>
       </c>
       <c r="X17">
-        <v>0.02367884916396554</v>
+        <v>0.06624626274899952</v>
       </c>
       <c r="Y17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Z17" t="s">
         <v>47</v>
       </c>
       <c r="AA17">
-        <v>0.6363588516746411</v>
+        <v>0.6249090909090909</v>
       </c>
       <c r="AB17">
-        <v>0.1108183969750727</v>
+        <v>0.04878340505235926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>